<commit_message>
Added Tables for competing frameworks
</commit_message>
<xml_diff>
--- a/Deliverables/20221020SpecsFrameworks.xlsx
+++ b/Deliverables/20221020SpecsFrameworks.xlsx
@@ -8,25 +8,37 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\boiss\Desktop\Cours\PR&amp;D Deep Agora\Deep-Agora_DOC\Deliverables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A346A926-B0D3-4CDA-B5F1-0DE4E1E7A5F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{291F08E1-1D3C-498A-908F-6D3613AD41B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Competing Frameworks" sheetId="1" r:id="rId1"/>
-    <sheet name="Desired Features" sheetId="2" r:id="rId2"/>
+    <sheet name="Features" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="38">
   <si>
     <r>
       <rPr>
@@ -51,9 +63,6 @@
     </r>
   </si>
   <si>
-    <t>Table of the competing Frameworks</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -100,18 +109,9 @@
     </r>
   </si>
   <si>
-    <t>Character extraction</t>
-  </si>
-  <si>
-    <t>Pixel categorisation</t>
-  </si>
-  <si>
     <t>Ornament extraction</t>
   </si>
   <si>
-    <t>XML</t>
-  </si>
-  <si>
     <t>ALTO XML</t>
   </si>
   <si>
@@ -133,12 +133,6 @@
     <t>Documentation</t>
   </si>
   <si>
-    <t>PyTorch</t>
-  </si>
-  <si>
-    <t>Tensorflow</t>
-  </si>
-  <si>
     <t>Segmentation down to characters</t>
   </si>
   <si>
@@ -169,6 +163,144 @@
     <t>dhSegment</t>
   </si>
   <si>
+    <t>The annotated images in label folder are usually RGB images with the regions to segment annotated with a specific color.
+We suppose this is how the CESR annotated them so it should take this input data.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Each training sample consists in an image of a document and its corresponding parts to be predicted.
+Additionally, a text file encoding the RGB values of the classes needs to be provided. In this case if we want the classes ‘background’, ‘document’ and ‘photograph’ to be respectively classes 0, 1, and 2 we need to encode their color line-by-line:
+0 255 0
+255 0 0
+0 0 255
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="3" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Click for more info.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Agora must specifically extract the characters. In this way, they can be dealt with much more easily. As this can be more difficult on older document frameworks, some of them only extract baselines. In our case, the segmentation should be done down to the characters, not just the baselines.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="3" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Click for more info.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Frameworks designed for Ancient Document Layout Analysis usually use additional features than others, in order to take into account broken characters, stains, poor paper quality, and so on.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="3" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Click for more info.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">In the case of handwritten documents, one or more characters, words or even lines tend to touch each other and are treated as the same content items.
+Therefore, the extraction of handwritten content items is impossible because too many of them touch each other.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="3" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Click for more info.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">In ancient document, are all types of EOC that are extremely valuable for their amount of historical information:
+- dropped capital letters
+- banners
+- illustrations (drawings/engravings)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="3" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Click for more info.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="3" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>It has been revealed that binarisation algorithms were not efficient enough in previous versions of Agora, so they will be avoided as a pre-processing requirement.</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="3" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Click for more info.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The user expressed the need to have an ALTO file as output of Agora. It is interpretable and well structured.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="3" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Click for more info.</t>
+    </r>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -188,15 +320,39 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> 1h</t>
-    </r>
+      <t xml:space="preserve"> 3h</t>
+    </r>
+  </si>
+  <si>
+    <t>The Deep-Agora project should be continued. Therefore, it would be better if the tools it uses were also pursued.</t>
+  </si>
+  <si>
+    <t>It helps to shorten the developer's adaptation phase.</t>
+  </si>
+  <si>
+    <t>Boxes detection compatible with handwritten text</t>
+  </si>
+  <si>
+    <t>Boxes may be difficult to position in the case of ancient documents, where characters may be broken or he text may be handwritten.</t>
+  </si>
+  <si>
+    <t>The purpose of box detection is to locate the EOCs in the image. It must be applied to characters, lines and ornaments in order to write their coordinates in the ALTO file.</t>
+  </si>
+  <si>
+    <t>Handle ancient document quality</t>
+  </si>
+  <si>
+    <t>SCORE</t>
+  </si>
+  <si>
+    <t>Table of the competing frameworks</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -212,6 +368,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="3" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="3" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -221,7 +400,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -255,11 +434,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -281,8 +474,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -561,161 +787,192 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O22"/>
+  <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="15" width="13.44140625" customWidth="1"/>
+    <col min="2" max="2" width="14.77734375" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="14.77734375" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="11" width="14.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="7"/>
       <c r="B8" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="I8" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="J8" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="K8" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="L8" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="K9" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="L9" s="20">
+        <f>COUNTA($B9:K9)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="18"/>
+      <c r="C10" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="J10" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="K10" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="L10" s="4">
+        <f>COUNTA($B10:K10)</f>
         <v>6</v>
       </c>
-      <c r="D8" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="H8" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="I8" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="J8" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="K8" s="8" t="s">
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="K11" s="18"/>
+      <c r="L11" s="4">
+        <f>COUNTA($B11:K11)</f>
         <v>7</v>
       </c>
-      <c r="L8" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="M8" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="N8" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="O8" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
-      <c r="O9" s="4"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="4"/>
-      <c r="O10" s="4"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
-      <c r="N11" s="4"/>
-      <c r="O11" s="4"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
@@ -743,204 +1000,195 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95DE170E-BC48-46B5-A05B-9B54249D65E4}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="26.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="13.77734375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="69.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.77734375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="33.33203125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="33.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="7"/>
       <c r="B1" s="8" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="5"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>26</v>
+      </c>
       <c r="C2" s="5" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="4"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="4"/>
-    </row>
-    <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="5"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="13"/>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="10"/>
+      <c r="F3" s="13"/>
+    </row>
+    <row r="4" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>24</v>
+      </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="4"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="10"/>
+      <c r="F4" s="13"/>
+    </row>
+    <row r="5" spans="1:8" ht="144" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="13"/>
+    </row>
+    <row r="6" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="13"/>
+    </row>
+    <row r="8" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="10"/>
+      <c r="F8" s="13"/>
+    </row>
+    <row r="9" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="5"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="13"/>
+    </row>
+    <row r="10" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="10"/>
+      <c r="F10" s="13"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="4"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="4"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="4"/>
-    </row>
-    <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="4"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="4"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="4"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="5"/>
+      <c r="B11" s="16" t="s">
+        <v>31</v>
+      </c>
       <c r="C11" s="5"/>
       <c r="D11" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" s="5"/>
-      <c r="F11" s="4"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" s="5"/>
-      <c r="F12" s="4"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E13" s="5"/>
-      <c r="F13" s="4"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E14" s="5"/>
-      <c r="F14" s="4"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E15" s="5"/>
-      <c r="F15" s="4"/>
+        <v>14</v>
+      </c>
+      <c r="E11" s="10"/>
+      <c r="F11" s="13"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" location="II.VISUAL" display="https://github.com/theo-boi/Deep-Agora_DOC/blob/main/Meeting minutes/221006PresentationExistingSystem.md - II.VISUAL" xr:uid="{2B92E580-90E9-4286-A6B7-C20523A3B02A}"/>
+    <hyperlink ref="B3" r:id="rId2" location="II.TOCHANGE" display="https://github.com/theo-boi/Deep-Agora_DOC/blob/main/Meeting minutes/220922Needs.md - II.TOCHANGE" xr:uid="{4A4002E3-051C-40E5-8F8E-3C3D60F5005E}"/>
+    <hyperlink ref="B4" r:id="rId3" location="II.FRAMEWORKS" display="https://github.com/theo-boi/Deep-Agora_DOC/blob/main/Meeting minutes/221019SpecifsOutline.md - II.FRAMEWORKS" xr:uid="{BA8E9823-5699-4A84-BC52-B71F98487593}"/>
+    <hyperlink ref="B5" r:id="rId4" display="Click for more info." xr:uid="{19EF7504-3833-4307-878E-FD77FCCBB572}"/>
+    <hyperlink ref="B9" r:id="rId5" location="III." display="https://github.com/theo-boi/Deep-Agora_DOC/blob/main/Meeting minutes/220922Needs.md - III." xr:uid="{05EC0E8B-5243-45FA-B51E-09181402CE89}"/>
+    <hyperlink ref="B8" r:id="rId6" location="II.TOCHANGE" display="https://github.com/theo-boi/Deep-Agora_DOC/blob/main/Meeting minutes/220922Needs.md - II.TOCHANGE" xr:uid="{D60202A9-9113-4A09-8EF8-017CF3BF1AF5}"/>
+    <hyperlink ref="B7" r:id="rId7" location="II.INPUTS" display="Agora must specifically extract the characters. In this way, they can be dealt with much more easily. As this can be more difficult on older document frameworks, some of them only extract baselines. In our case, the segmentation should be done down to the characters, not just the baselines." xr:uid="{42B74197-1C95-408C-94A1-8AF4341B206B}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix Wrong link for ALTO XML
</commit_message>
<xml_diff>
--- a/Deliverables/20221020SpecsFrameworks.xlsx
+++ b/Deliverables/20221020SpecsFrameworks.xlsx
@@ -8,16 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\boiss\Desktop\Cours\PR&amp;D Deep Agora\Deep-Agora_DOC\Deliverables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{291F08E1-1D3C-498A-908F-6D3613AD41B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4E14466-2251-4C68-9151-1D1D443F21CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Competing Frameworks" sheetId="1" r:id="rId1"/>
     <sheet name="Features" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -789,8 +788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1002,8 +1001,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95DE170E-BC48-46B5-A05B-9B54249D65E4}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1184,7 +1183,7 @@
     <hyperlink ref="B3" r:id="rId2" location="II.TOCHANGE" display="https://github.com/theo-boi/Deep-Agora_DOC/blob/main/Meeting minutes/220922Needs.md - II.TOCHANGE" xr:uid="{4A4002E3-051C-40E5-8F8E-3C3D60F5005E}"/>
     <hyperlink ref="B4" r:id="rId3" location="II.FRAMEWORKS" display="https://github.com/theo-boi/Deep-Agora_DOC/blob/main/Meeting minutes/221019SpecifsOutline.md - II.FRAMEWORKS" xr:uid="{BA8E9823-5699-4A84-BC52-B71F98487593}"/>
     <hyperlink ref="B5" r:id="rId4" display="Click for more info." xr:uid="{19EF7504-3833-4307-878E-FD77FCCBB572}"/>
-    <hyperlink ref="B9" r:id="rId5" location="III." display="https://github.com/theo-boi/Deep-Agora_DOC/blob/main/Meeting minutes/220922Needs.md - III." xr:uid="{05EC0E8B-5243-45FA-B51E-09181402CE89}"/>
+    <hyperlink ref="B9" r:id="rId5" location="III." display="https://github.com/theo-boi/Deep-Agora_DOC/blob/main/Meeting minutes/221012RETRO.md - III." xr:uid="{05EC0E8B-5243-45FA-B51E-09181402CE89}"/>
     <hyperlink ref="B8" r:id="rId6" location="II.TOCHANGE" display="https://github.com/theo-boi/Deep-Agora_DOC/blob/main/Meeting minutes/220922Needs.md - II.TOCHANGE" xr:uid="{D60202A9-9113-4A09-8EF8-017CF3BF1AF5}"/>
     <hyperlink ref="B7" r:id="rId7" location="II.INPUTS" display="Agora must specifically extract the characters. In this way, they can be dealt with much more easily. As this can be more difficult on older document frameworks, some of them only extract baselines. In our case, the segmentation should be done down to the characters, not just the baselines." xr:uid="{42B74197-1C95-408C-94A1-8AF4341B206B}"/>
   </hyperlinks>

</xml_diff>

<commit_message>
Added time spent to Specs Frameworks Table
</commit_message>
<xml_diff>
--- a/Deliverables/20221020SpecsFrameworks.xlsx
+++ b/Deliverables/20221020SpecsFrameworks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\boiss\Desktop\Cours\PR&amp;D Deep Agora\Deep-Agora_DOC\Deliverables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4E14466-2251-4C68-9151-1D1D443F21CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D763C022-2359-4EB4-8C46-AF5115EE3BF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Competing Frameworks" sheetId="1" r:id="rId1"/>
@@ -300,6 +300,30 @@
     </r>
   </si>
   <si>
+    <t>The Deep-Agora project should be continued. Therefore, it would be better if the tools it uses were also pursued.</t>
+  </si>
+  <si>
+    <t>It helps to shorten the developer's adaptation phase.</t>
+  </si>
+  <si>
+    <t>Boxes detection compatible with handwritten text</t>
+  </si>
+  <si>
+    <t>Boxes may be difficult to position in the case of ancient documents, where characters may be broken or he text may be handwritten.</t>
+  </si>
+  <si>
+    <t>The purpose of box detection is to locate the EOCs in the image. It must be applied to characters, lines and ornaments in order to write their coordinates in the ALTO file.</t>
+  </si>
+  <si>
+    <t>Handle ancient document quality</t>
+  </si>
+  <si>
+    <t>SCORE</t>
+  </si>
+  <si>
+    <t>Table of the competing frameworks</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -319,32 +343,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> 3h</t>
-    </r>
-  </si>
-  <si>
-    <t>The Deep-Agora project should be continued. Therefore, it would be better if the tools it uses were also pursued.</t>
-  </si>
-  <si>
-    <t>It helps to shorten the developer's adaptation phase.</t>
-  </si>
-  <si>
-    <t>Boxes detection compatible with handwritten text</t>
-  </si>
-  <si>
-    <t>Boxes may be difficult to position in the case of ancient documents, where characters may be broken or he text may be handwritten.</t>
-  </si>
-  <si>
-    <t>The purpose of box detection is to locate the EOCs in the image. It must be applied to characters, lines and ornaments in order to write their coordinates in the ALTO file.</t>
-  </si>
-  <si>
-    <t>Handle ancient document quality</t>
-  </si>
-  <si>
-    <t>SCORE</t>
-  </si>
-  <si>
-    <t>Table of the competing frameworks</t>
+      <t xml:space="preserve"> 4h</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -788,8 +788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -804,7 +804,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
@@ -822,7 +822,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
@@ -845,7 +845,7 @@
         <v>5</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G8" s="8" t="s">
         <v>11</v>
@@ -863,7 +863,7 @@
         <v>10</v>
       </c>
       <c r="L8" s="19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
@@ -1001,7 +1001,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95DE170E-BC48-46B5-A05B-9B54249D65E4}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -1063,7 +1063,7 @@
     </row>
     <row r="4" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>24</v>
@@ -1093,10 +1093,10 @@
     </row>
     <row r="6" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5" t="s">
@@ -1104,7 +1104,7 @@
       </c>
       <c r="E6" s="10"/>
       <c r="F6" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="72" x14ac:dyDescent="0.3">
@@ -1154,7 +1154,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5" t="s">
@@ -1168,7 +1168,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="5" t="s">

</xml_diff>

<commit_message>
Update according to the state of the art
</commit_message>
<xml_diff>
--- a/Deliverables/20221020SpecsFrameworks.xlsx
+++ b/Deliverables/20221020SpecsFrameworks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\boiss\Desktop\Cours\PR&amp;D Deep Agora\Deep-Agora_DOC\Deliverables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D730B007-81FE-4BCC-8779-D126225C6999}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91385532-6B4F-4F09-9543-373CCD0B004F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="55">
   <si>
     <r>
       <rPr>
@@ -211,26 +211,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">In ancient document, are all types of EOC that are extremely valuable for their amount of historical information:
-- dropped capital letters
-- banners
-- illustrations (drawings/engravings)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="3" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Click for more info.</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <rPr>
         <sz val="11"/>
         <color theme="3" tint="-0.499984740745262"/>
@@ -367,6 +347,38 @@
     <t>Character-level segmentation</t>
   </si>
   <si>
+    <t>Baseline detection methods use a simple post-processing step that consists of filtering connected components. In the case of character-level segmentation and handwritten text, this method is ineffective.</t>
+  </si>
+  <si>
+    <t>Other methods than grouping connected black pixels exist to post-process the predictions.</t>
+  </si>
+  <si>
+    <t>Post-processing allows filtering other than by CC</t>
+  </si>
+  <si>
+    <t>Most models predict baselines, not the characters themselves. The use of a detection method based on connected components prevents any post-processing on handwritten characters.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">In ancient document, are all types of EOC that are extremely valuable for their amount of historical information:
+- initial capitals
+- banners
+- illustrations (drawings/engravings)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="3" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Click for more info.</t>
+    </r>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -386,20 +398,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> 2.0</t>
-    </r>
-  </si>
-  <si>
-    <t>Baseline detection methods use a simple post-processing step that consists of filtering connected components. In the case of character-level segmentation and handwritten text, this method is ineffective.</t>
-  </si>
-  <si>
-    <t>Other methods than grouping connected black pixels exist to post-process the predictions.</t>
-  </si>
-  <si>
-    <t>Post-processing allows filtering other than by CC</t>
-  </si>
-  <si>
-    <t>Most models predict baselines, not the characters themselves. The use of a detection method based on connected components prevents any post-processing on handwritten characters.</t>
+      <t xml:space="preserve"> 2.2</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -539,7 +539,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -622,6 +622,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -906,7 +909,7 @@
   <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -923,7 +926,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
@@ -941,12 +944,12 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
@@ -961,16 +964,16 @@
         <v>4</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F8" s="19" t="s">
         <v>3</v>
       </c>
       <c r="G8" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H8" s="19" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I8" s="19" t="s">
         <v>6</v>
@@ -982,7 +985,7 @@
         <v>8</v>
       </c>
       <c r="L8" s="17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
@@ -1080,7 +1083,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="27" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B12" s="28" t="s">
         <v>11</v>
@@ -1099,10 +1102,12 @@
         <v>11</v>
       </c>
       <c r="J12" s="26"/>
-      <c r="K12" s="26"/>
+      <c r="K12" s="32" t="s">
+        <v>11</v>
+      </c>
       <c r="L12" s="26">
         <f>COUNTA($B12:K12)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
@@ -1160,9 +1165,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95DE170E-BC48-46B5-A05B-9B54249D65E4}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1196,17 +1199,17 @@
         <v>2</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H2" s="2"/>
     </row>
@@ -1222,10 +1225,10 @@
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="144" x14ac:dyDescent="0.3">
@@ -1243,12 +1246,12 @@
         <v>18</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B5" s="13" t="s">
         <v>20</v>
@@ -1258,10 +1261,10 @@
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -1269,22 +1272,22 @@
         <v>3</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>21</v>
@@ -1294,28 +1297,28 @@
         <v>11</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E8" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="F8" s="10" t="s">
         <v>52</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
@@ -1323,17 +1326,17 @@
         <v>6</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -1341,17 +1344,17 @@
         <v>7</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -1359,17 +1362,17 @@
         <v>8</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C11" s="22"/>
       <c r="D11" s="22" t="s">
         <v>11</v>
       </c>
       <c r="E11" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" s="23" t="s">
         <v>38</v>
-      </c>
-      <c r="F11" s="23" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added note for datasets
</commit_message>
<xml_diff>
--- a/Deliverables/20221020SpecsFrameworks.xlsx
+++ b/Deliverables/20221020SpecsFrameworks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\boiss\Desktop\Cours\PR&amp;D Deep Agora\Deep-Agora_DOC\Deliverables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91385532-6B4F-4F09-9543-373CCD0B004F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB13A833-6FB3-410A-9ADA-E9A728BF80AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Competing Frameworks" sheetId="1" r:id="rId1"/>
@@ -159,23 +159,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Agora must specifically extract the characters. In this way, they can be dealt with much more easily. As this can be more difficult on older document frameworks, some of them only extract baselines. In our case, the segmentation should be done down to the characters, not just the baselines.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="3" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Click for more info.</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">Frameworks designed for Ancient Document Layout Analysis usually use additional features than others, in order to take into account broken characters, stains, poor paper quality, and so on.
 </t>
     </r>
@@ -347,16 +330,10 @@
     <t>Character-level segmentation</t>
   </si>
   <si>
-    <t>Baseline detection methods use a simple post-processing step that consists of filtering connected components. In the case of character-level segmentation and handwritten text, this method is ineffective.</t>
-  </si>
-  <si>
     <t>Other methods than grouping connected black pixels exist to post-process the predictions.</t>
   </si>
   <si>
     <t>Post-processing allows filtering other than by CC</t>
-  </si>
-  <si>
-    <t>Most models predict baselines, not the characters themselves. The use of a detection method based on connected components prevents any post-processing on handwritten characters.</t>
   </si>
   <si>
     <r>
@@ -400,6 +377,29 @@
       </rPr>
       <t xml:space="preserve"> 2.2</t>
     </r>
+  </si>
+  <si>
+    <t>Most models predict baselines, not the characters themselves because their detection method is based on connected components which prevents any post-processing on handwritten characters.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Agora must specifically extract the characters. In this way, they can be dealt with much more easily. As ancient document analysis frameworks are usually designed for further OCR opperations, they only extract baselines. In our case, the segmentation should be done down to the characters, not just the baselines.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="3" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Click for more info.</t>
+    </r>
+  </si>
+  <si>
+    <t>Segmentation methods usually use a simple post-processing step that consists of filtering connected components. In the case of character-level segmentation in handwritten text, this method is ineffective.</t>
   </si>
 </sst>
 </file>
@@ -908,9 +908,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -926,7 +924,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
@@ -944,12 +942,12 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
@@ -964,16 +962,16 @@
         <v>4</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F8" s="19" t="s">
         <v>3</v>
       </c>
       <c r="G8" s="19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H8" s="19" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I8" s="19" t="s">
         <v>6</v>
@@ -985,7 +983,7 @@
         <v>8</v>
       </c>
       <c r="L8" s="17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
@@ -1083,7 +1081,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B12" s="28" t="s">
         <v>11</v>
@@ -1199,17 +1197,17 @@
         <v>2</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H2" s="2"/>
     </row>
@@ -1218,17 +1216,17 @@
         <v>5</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="144" x14ac:dyDescent="0.3">
@@ -1246,25 +1244,25 @@
         <v>18</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>20</v>
+        <v>53</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -1272,50 +1270,50 @@
         <v>3</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F8" s="10" t="s">
         <v>52</v>
@@ -1326,17 +1324,17 @@
         <v>6</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -1344,17 +1342,17 @@
         <v>7</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -1362,17 +1360,17 @@
         <v>8</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C11" s="22"/>
       <c r="D11" s="22" t="s">
         <v>11</v>
       </c>
       <c r="E11" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" s="23" t="s">
         <v>37</v>
-      </c>
-      <c r="F11" s="23" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished Specifications and Analysis
</commit_message>
<xml_diff>
--- a/Deliverables/20221020SpecsFrameworks.xlsx
+++ b/Deliverables/20221020SpecsFrameworks.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\boiss\Desktop\Cours\PR&amp;D Deep Agora\Deep-Agora_DOC\Deliverables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B18E8703-4C67-4821-9085-E9E8DBCD8228}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C50225D8-A61B-4B87-A209-30F774EE278A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -156,23 +156,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Frameworks designed for Ancient Document Layout Analysis usually use additional features than others, in order to take into account broken characters, stains, poor paper quality, and so on.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="3" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Click for more info.</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">In the case of handwritten documents, one or more characters, words or even lines tend to touch each other and are treated as the same content items.
 Therefore, the extraction of handwritten content items is impossible because too many of them touch each other.
 </t>
@@ -310,11 +293,23 @@
     <t>Post-processing allows filtering other than by CC</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">In ancient document, are all types of EOC that are extremely valuable for their amount of historical information:
-- initial capitals
-- banners
-- illustrations (drawings/engravings)
+    <t>Most models predict baselines, not the characters themselves because their detection method is based on connected components which prevents any post-processing on handwritten characters.</t>
+  </si>
+  <si>
+    <t>Segmentation methods usually use a simple post-processing step that consists of filtering connected components. In the case of character-level segmentation in handwritten text, this method is ineffective.</t>
+  </si>
+  <si>
+    <t>Line-level segmentation</t>
+  </si>
+  <si>
+    <t>In our case, the segmentation could be done down to the characters, not just the text lines, if the client changes their mind.</t>
+  </si>
+  <si>
+    <t>Agora must extract text lines in text blocks. In this way, they can be dealt with by usual OCRs or used in order to extract new policies. As ancient document analysis frameworks are usually designed for further OCR operations, they only extract text lines.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Agora may extract the characters. In this way, they can be dealt with much more easily by RETRO.
 </t>
     </r>
     <r>
@@ -330,23 +325,81 @@
     </r>
   </si>
   <si>
-    <t>Most models predict baselines, not the characters themselves because their detection method is based on connected components which prevents any post-processing on handwritten characters.</t>
-  </si>
-  <si>
-    <t>Segmentation methods usually use a simple post-processing step that consists of filtering connected components. In the case of character-level segmentation in handwritten text, this method is ineffective.</t>
-  </si>
-  <si>
-    <t>Line-level segmentation</t>
-  </si>
-  <si>
-    <t>In our case, the segmentation could be done down to the characters, not just the text lines, if the client changes their mind.</t>
-  </si>
-  <si>
-    <t>Agora must extract text lines in text blocks. In this way, they can be dealt with by usual OCRs or used in order to extract new policies. As ancient document analysis frameworks are usually designed for further OCR operations, they only extract text lines.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Agora may extract the characters. In this way, they can be dealt with much more easily by RETRO.
+    <t>Decoration segmentation</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Version:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 3.0</t>
+    </r>
+  </si>
+  <si>
+    <t>Average of the ratios of the feature point for the library to the feature points for other libraries.</t>
+  </si>
+  <si>
+    <t>The ratio of the library's points to those of others.</t>
+  </si>
+  <si>
+    <t>Mean of the two previous scores (%).</t>
+  </si>
+  <si>
+    <t>Score relative to the line</t>
+  </si>
+  <si>
+    <t>Score relative to the columns</t>
+  </si>
+  <si>
+    <t>The right library has specific advantages.</t>
+  </si>
+  <si>
+    <t>The right library has more many advantages.</t>
+  </si>
+  <si>
+    <t>The right library has many and specific advantages.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Time spent:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 8h</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Frameworks designed for Historical Document Layout Analysis usually use additional features than others, in order to take into account broken characters, stains, poor paper quality, and so on.
 </t>
     </r>
     <r>
@@ -362,76 +415,23 @@
     </r>
   </si>
   <si>
-    <t>Decoration segmentation</t>
-  </si>
-  <si>
+    <r>
+      <t xml:space="preserve">In ancient documents are all types of EOC that are extremely valuable for their amount of historical information:
+- initial capitals
+- banners
+- illustrations (drawings/engravings)
+</t>
+    </r>
     <r>
       <rPr>
-        <b/>
+        <u/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color theme="3" tint="-0.499984740745262"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Version:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 3.0</t>
-    </r>
-  </si>
-  <si>
-    <t>Average of the ratios of the feature point for the library to the feature points for other libraries.</t>
-  </si>
-  <si>
-    <t>The ratio of the library's points to those of others.</t>
-  </si>
-  <si>
-    <t>Mean of the two previous scores (%).</t>
-  </si>
-  <si>
-    <t>Score relative to the line</t>
-  </si>
-  <si>
-    <t>Score relative to the columns</t>
-  </si>
-  <si>
-    <t>The right library has specific advantages.</t>
-  </si>
-  <si>
-    <t>The right library has more many advantages.</t>
-  </si>
-  <si>
-    <t>The right library has many and specific advantages.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Time spent:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 8h</t>
+      <t>Click for more info.</t>
     </r>
   </si>
 </sst>
@@ -611,7 +611,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -648,10 +648,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -664,17 +664,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -684,14 +684,11 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -700,29 +697,20 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1003,11 +991,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.77734375" customWidth="1"/>
@@ -1021,7 +1007,7 @@
   <sheetData>
     <row r="1" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
@@ -1039,57 +1025,57 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="7"/>
-      <c r="B8" s="40" t="s">
+      <c r="B8" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="36" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" s="36" t="s">
+        <v>53</v>
+      </c>
+      <c r="F8" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="G8" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="H8" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="I8" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="J8" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="K8" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="L8" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="M8" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="N8" s="33" t="s">
+        <v>59</v>
+      </c>
+      <c r="O8" s="37" t="s">
         <v>25</v>
-      </c>
-      <c r="C8" s="40" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="E8" s="40" t="s">
-        <v>55</v>
-      </c>
-      <c r="F8" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="G8" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="H8" s="40" t="s">
-        <v>5</v>
-      </c>
-      <c r="I8" s="40" t="s">
-        <v>2</v>
-      </c>
-      <c r="J8" s="40" t="s">
-        <v>3</v>
-      </c>
-      <c r="K8" s="40" t="s">
-        <v>6</v>
-      </c>
-      <c r="L8" s="40" t="s">
-        <v>7</v>
-      </c>
-      <c r="M8" s="34" t="s">
-        <v>60</v>
-      </c>
-      <c r="N8" s="34" t="s">
-        <v>61</v>
-      </c>
-      <c r="O8" s="41" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
@@ -1104,7 +1090,7 @@
       <c r="E9" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="35"/>
+      <c r="F9" s="16"/>
       <c r="G9" s="16"/>
       <c r="H9" s="16" t="s">
         <v>10</v>
@@ -1129,7 +1115,7 @@
         <f>ROUND((COUNTA(B9)/COUNTA($B$9:$B$12)+COUNTA(C9)/COUNTA($C$9:$C$12)+COUNTA(D9)/COUNTA($D$9:$D$12)+COUNTA(E9)/COUNTA($E$9:$E$12)+COUNTA(H9)/COUNTA($H$9:$H$12)+(COUNTA(I9)/COUNTA($I$9:$I$12)+COUNTA(J9)/COUNTA($J9:$J$12)+COUNTA(K9)/COUNTA($K$9:$K$12)+COUNTA(L9)/COUNTA($L$9:$L$12))/2)/9,2)*100</f>
         <v>18</v>
       </c>
-      <c r="O9" s="37">
+      <c r="O9" s="34">
         <f>ROUND(AVERAGE(M9:N9),0)</f>
         <v>26</v>
       </c>
@@ -1148,7 +1134,7 @@
         <v>10</v>
       </c>
       <c r="E10" s="16"/>
-      <c r="F10" s="35"/>
+      <c r="F10" s="16"/>
       <c r="G10" s="16"/>
       <c r="H10" s="16"/>
       <c r="I10" s="16" t="s">
@@ -1171,7 +1157,7 @@
         <f>ROUND((COUNTA(B10)/COUNTA($B$9:$B$12)+COUNTA(C10)/COUNTA($C$9:$C$12)+COUNTA(D10)/COUNTA($D$9:$D$12)+COUNTA(E10)/COUNTA($E$9:$E$12)+COUNTA(H10)/COUNTA($H$9:$H$12)+(COUNTA(I10)/COUNTA($I$9:$I$12)+COUNTA(J10)/COUNTA($J10:$J$12)+COUNTA(K10)/COUNTA($K$9:$K$12)+COUNTA(L10)/COUNTA($L$9:$L$12))/2)/9,2)*100</f>
         <v>20</v>
       </c>
-      <c r="O10" s="37">
+      <c r="O10" s="34">
         <f t="shared" ref="O10:O12" si="0">ROUND(AVERAGE(M10:N10),0)</f>
         <v>27</v>
       </c>
@@ -1215,14 +1201,14 @@
         <f>ROUND((COUNTA(B11)/COUNTA($B$9:$B$12)+COUNTA(C11)/COUNTA($C$9:$C$12)+COUNTA(D11)/COUNTA($D$9:$D$12)+COUNTA(E11)/COUNTA($E$9:$E$12)+COUNTA(H11)/COUNTA($H$9:$H$12)+(COUNTA(I11)/COUNTA($I$9:$I$12)+COUNTA(J11)/COUNTA($J11:$J$12)+COUNTA(K11)/COUNTA($K$9:$K$12)+COUNTA(L11)/COUNTA($L$9:$L$12))/2)/9,2)*100</f>
         <v>24</v>
       </c>
-      <c r="O11" s="38">
+      <c r="O11" s="35">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B12" s="24" t="s">
         <v>10</v>
@@ -1234,7 +1220,7 @@
       <c r="E12" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="36"/>
+      <c r="F12" s="24"/>
       <c r="G12" s="22"/>
       <c r="H12" s="24" t="s">
         <v>10</v>
@@ -1244,7 +1230,7 @@
         <v>10</v>
       </c>
       <c r="K12" s="22"/>
-      <c r="L12" s="28" t="s">
+      <c r="L12" s="24" t="s">
         <v>10</v>
       </c>
       <c r="M12" s="22">
@@ -1317,7 +1303,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="26.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="69.44140625" style="3" bestFit="1" customWidth="1"/>
@@ -1346,20 +1332,20 @@
     </row>
     <row r="2" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>19</v>
+        <v>64</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5" t="s">
         <v>10</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="72" x14ac:dyDescent="0.3">
@@ -1367,88 +1353,88 @@
         <v>4</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>53</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F4" s="10"/>
     </row>
     <row r="5" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>48</v>
+        <v>65</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H5" s="2"/>
     </row>
     <row r="6" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A6" s="32" t="s">
-        <v>45</v>
+      <c r="A6" s="31" t="s">
+        <v>44</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="72" x14ac:dyDescent="0.3">
-      <c r="A7" s="9" t="s">
-        <v>47</v>
+      <c r="A7" s="31" t="s">
+        <v>46</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5" t="s">
         <v>10</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
@@ -1456,17 +1442,17 @@
         <v>5</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5" t="s">
         <v>10</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -1474,17 +1460,17 @@
         <v>2</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="144" x14ac:dyDescent="0.3">
@@ -1502,7 +1488,7 @@
         <v>17</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -1510,76 +1496,76 @@
         <v>6</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="5" t="s">
         <v>10</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="30" t="s">
-        <v>24</v>
+      <c r="B12" s="29" t="s">
+        <v>23</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="5" t="s">
         <v>10</v>
       </c>
       <c r="E12" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="F12" s="10" t="s">
-        <v>36</v>
-      </c>
     </row>
     <row r="13" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="32" t="s">
-        <v>60</v>
-      </c>
-      <c r="B13" s="39" t="s">
+      <c r="A13" s="31" t="s">
         <v>58</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>56</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F13" s="10"/>
     </row>
     <row r="14" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="32" t="s">
-        <v>61</v>
-      </c>
-      <c r="B14" s="39" t="s">
-        <v>57</v>
+      <c r="A14" s="31" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>55</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F14" s="10"/>
     </row>
     <row r="15" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="33" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="31" t="s">
-        <v>59</v>
+      <c r="A15" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="30" t="s">
+        <v>57</v>
       </c>
       <c r="C15" s="18"/>
       <c r="D15" s="18"/>
       <c r="E15" s="19" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F15" s="19"/>
     </row>

</xml_diff>